<commit_message>
Added Docs for v0.2
</commit_message>
<xml_diff>
--- a/PCB/BOM.xlsx
+++ b/PCB/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="11070"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="16230"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PartType-TeensyBat" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="273">
   <si>
     <t>Comment</t>
   </si>
@@ -207,24 +207,6 @@
     <t>http://octopart.com/erj-8enf2202v-panasonic-10475275</t>
   </si>
   <si>
-    <t>100k</t>
-  </si>
-  <si>
-    <t>Thick Film Resistors - SMD 1206 100Kohms 1% Tolerance</t>
-  </si>
-  <si>
-    <t>R23</t>
-  </si>
-  <si>
-    <t>CMP-3656152-2</t>
-  </si>
-  <si>
-    <t>5cd296951d0c8315</t>
-  </si>
-  <si>
-    <t>https://octopart.com/erj-8enf1003v-panasonic-55403704</t>
-  </si>
-  <si>
     <t>4.7k</t>
   </si>
   <si>
@@ -766,9 +748,6 @@
   </si>
   <si>
     <t>https://octopart.com/12065c473kat2a-avx+interconnect+%2F+elco-39667180</t>
-  </si>
-  <si>
-    <t>C15</t>
   </si>
   <si>
     <t>AVX Interconnect / Elco 12065C105KAT2A</t>
@@ -1208,7 +1187,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G77"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1611,117 +1590,117 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="D18" s="2" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="F18" s="3">
         <v>1</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="3">
-        <v>1</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="D20" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F20" s="3">
         <v>1</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="D21" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="F21" s="3">
         <v>1</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="F22" s="3">
         <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1732,7 +1711,7 @@
         <v>57</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>59</v>
@@ -1749,25 +1728,25 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="3">
+        <v>1</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F24" s="3">
-        <v>1</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1795,94 +1774,94 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="D26" s="2" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="F26" s="3">
         <v>1</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F27" s="3">
+        <v>1</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F27" s="3">
-        <v>1</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="D28" s="2" t="s">
-        <v>107</v>
+        <v>71</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
       <c r="F28" s="3">
         <v>1</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="F29" s="3">
         <v>1</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1893,7 +1872,7 @@
         <v>92</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>94</v>
@@ -1910,25 +1889,25 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F31" s="3">
+        <v>1</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F31" s="3">
-        <v>1</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1936,137 +1915,137 @@
         <v>113</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>115</v>
-      </c>
       <c r="D32" s="2" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>117</v>
+        <v>66</v>
       </c>
       <c r="F32" s="3">
         <v>1</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>118</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C33" s="2" t="s">
+      <c r="F33" s="3">
+        <v>1</v>
+      </c>
+      <c r="G33" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F33" s="3">
-        <v>1</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="D34" s="2" t="s">
-        <v>124</v>
+        <v>42</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>125</v>
+        <v>43</v>
       </c>
       <c r="F34" s="3">
         <v>1</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>126</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>40</v>
+        <v>123</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F35" s="3">
+        <v>1</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F35" s="3">
-        <v>1</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="D36" s="2" t="s">
-        <v>131</v>
+        <v>78</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>132</v>
+        <v>79</v>
       </c>
       <c r="F36" s="3">
         <v>1</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>133</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>82</v>
+        <v>130</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F37" s="3">
+        <v>1</v>
+      </c>
+      <c r="G37" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F37" s="3">
-        <v>1</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -2140,48 +2119,48 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="D41" s="2" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="F41" s="3">
         <v>1</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F42" s="3">
+        <v>1</v>
+      </c>
+      <c r="G42" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="F42" s="3">
-        <v>1</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -2255,48 +2234,48 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>180</v>
-      </c>
       <c r="D46" s="2" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="F46" s="3">
         <v>1</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C47" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="F47" s="3">
+        <v>1</v>
+      </c>
+      <c r="G47" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="F47" s="3">
-        <v>1</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -2347,48 +2326,48 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>199</v>
-      </c>
       <c r="D50" s="2" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="F50" s="3">
         <v>1</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C51" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="F51" s="3">
+        <v>1</v>
+      </c>
+      <c r="G51" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="F51" s="3">
-        <v>1</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2462,71 +2441,71 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>224</v>
-      </c>
       <c r="D55" s="2" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="F55" s="3">
         <v>1</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="F56" s="3">
         <v>1</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="C57" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="F57" s="3">
+        <v>1</v>
+      </c>
+      <c r="G57" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="F57" s="3">
-        <v>1</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -2554,48 +2533,48 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>238</v>
-      </c>
       <c r="D59" s="2" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="F59" s="3">
         <v>1</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="C60" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="F60" s="3">
+        <v>1</v>
+      </c>
+      <c r="G60" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="F60" s="3">
-        <v>1</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -2623,374 +2602,328 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>249</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="F62" s="3">
         <v>1</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>252</v>
-      </c>
       <c r="D63" s="2" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="F63" s="3">
         <v>1</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="F64" s="3">
         <v>1</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>250</v>
+        <v>216</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>251</v>
+        <v>217</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>253</v>
+        <v>219</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>254</v>
+        <v>220</v>
       </c>
       <c r="F65" s="3">
         <v>1</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>255</v>
+        <v>221</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="F66" s="3">
         <v>1</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>222</v>
+        <v>254</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>223</v>
+        <v>255</v>
       </c>
       <c r="C67" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="F67" s="3">
+        <v>1</v>
+      </c>
+      <c r="G67" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="F67" s="3">
-        <v>1</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>222</v>
+        <v>254</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>223</v>
+        <v>255</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>260</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>225</v>
+        <v>257</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>226</v>
+        <v>258</v>
       </c>
       <c r="F68" s="3">
         <v>1</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>227</v>
+        <v>259</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B69" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>263</v>
-      </c>
       <c r="D69" s="2" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="F69" s="3">
         <v>1</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C70" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="C70" s="2" t="s">
-        <v>267</v>
-      </c>
       <c r="D70" s="2" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="F70" s="3">
         <v>1</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="F71" s="3">
         <v>1</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="F72" s="3">
         <v>1</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="F73" s="3">
         <v>1</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="F74" s="3">
         <v>1</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="C75" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F75" s="3">
+        <v>1</v>
+      </c>
+      <c r="G75" s="2" t="s">
         <v>272</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="F75" s="3">
-        <v>1</v>
-      </c>
-      <c r="G75" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="F76" s="3">
-        <v>1</v>
-      </c>
-      <c r="G76" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="F77" s="3">
-        <v>1</v>
-      </c>
-      <c r="G77" s="2" t="s">
-        <v>279</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>